<commit_message>
Make data more uniform
</commit_message>
<xml_diff>
--- a/data/transaction_data-template.xlsx
+++ b/data/transaction_data-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41715674-BB0D-4CE6-9758-34BE3B4EC181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A59A3A4-E4A5-4D66-844D-F89DC9CBAF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21710" yWindow="-12910" windowWidth="21820" windowHeight="38020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CSVData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="1">
   <si>
     <t>[transaction ID]</t>
   </si>
@@ -875,7 +875,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,345 +889,333 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>44512</v>
-      </c>
-      <c r="B1" s="2">
-        <v>-710146.5</v>
+        <v>44540</v>
+      </c>
+      <c r="B1">
+        <v>-433.9</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2">
-        <v>164558.16</v>
+        <v>874704.66</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>44479</v>
-      </c>
-      <c r="B2">
-        <v>-433.9</v>
+      <c r="A2" s="3">
+        <v>44527</v>
+      </c>
+      <c r="B2" s="2">
+        <v>437569.28000000003</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>874704.66</v>
+        <v>875138.56000000006</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>44466</v>
-      </c>
-      <c r="B3" s="2">
+        <v>44491</v>
+      </c>
+      <c r="B3">
+        <v>-20.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>437569.28000000003</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>875138.56000000006</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>44461</v>
+        <v>44467</v>
       </c>
       <c r="B4">
-        <v>-20.5</v>
+        <v>-335</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>437569.28000000003</v>
+        <v>437589.78</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>44436</v>
-      </c>
-      <c r="B5">
-        <v>-335</v>
+        <v>44427</v>
+      </c>
+      <c r="B5" s="2">
+        <v>437924.78</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>437589.78</v>
+        <v>437924.78</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>44427</v>
-      </c>
-      <c r="B6" s="2">
-        <v>437924.78</v>
+        <v>44410</v>
+      </c>
+      <c r="B6">
+        <v>-101.1</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2">
-        <v>437924.78</v>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>44410</v>
-      </c>
-      <c r="B7">
-        <v>-101.1</v>
+        <v>44406</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-183171</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>101.1</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>44406</v>
+        <v>44383</v>
       </c>
       <c r="B8" s="2">
-        <v>-183171</v>
+        <v>91636.05</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D8">
-        <v>101.1</v>
+      <c r="D8" s="2">
+        <v>183272.1</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>44383</v>
+        <v>44372</v>
       </c>
       <c r="B9" s="2">
+        <v>13090.86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
         <v>91636.05</v>
-      </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>183272.1</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>44372</v>
+        <v>44366</v>
       </c>
       <c r="B10" s="2">
-        <v>13090.86</v>
+        <v>-2834.5</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2">
-        <v>91636.05</v>
+        <v>78545.19</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>44366</v>
+        <v>44359</v>
       </c>
       <c r="B11" s="2">
-        <v>-2834.5</v>
+        <v>20344.919999999998</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>78545.19</v>
+        <v>81379.69</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>44359</v>
+        <v>44355</v>
       </c>
       <c r="B12" s="2">
-        <v>20344.919999999998</v>
+        <v>-125302.39999999999</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2">
-        <v>81379.69</v>
+        <v>61034.77</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>44355</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-125302.39999999999</v>
+        <v>44311</v>
+      </c>
+      <c r="B13">
+        <v>-252.05</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2">
-        <v>61034.77</v>
+        <v>186337.17</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>44311</v>
-      </c>
-      <c r="B14">
-        <v>-252.05</v>
+        <v>44308</v>
+      </c>
+      <c r="B14" s="2">
+        <v>46647.31</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <v>186337.17</v>
+        <v>186589.22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>44308</v>
+        <v>44298</v>
       </c>
       <c r="B15" s="2">
-        <v>46647.31</v>
+        <v>23323.65</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2">
-        <v>186589.22</v>
+        <v>139941.92000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>44298</v>
+        <v>44282</v>
       </c>
       <c r="B16" s="2">
-        <v>23323.65</v>
+        <v>14577.28</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2">
-        <v>139941.92000000001</v>
+        <v>116618.27</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>44282</v>
+        <v>44251</v>
       </c>
       <c r="B17" s="2">
-        <v>14577.28</v>
+        <v>51020.5</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>116618.27</v>
+        <v>102040.99</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>44251</v>
-      </c>
-      <c r="B18" s="2">
+        <v>44248</v>
+      </c>
+      <c r="B18">
+        <v>-2.78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
         <v>51020.5</v>
       </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>102040.99</v>
-      </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>44248</v>
-      </c>
-      <c r="B19">
-        <v>-2.78</v>
+      <c r="A19" s="1">
+        <v>44244</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-300660</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <v>51020.5</v>
+        <v>51023.28</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44244</v>
+        <v>44240</v>
       </c>
       <c r="B20" s="2">
-        <v>-300660</v>
+        <v>87920.82</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <v>51023.28</v>
+        <v>351683.28</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44240</v>
+        <v>44231</v>
       </c>
       <c r="B21" s="2">
-        <v>87920.82</v>
+        <v>26376.25</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2">
-        <v>351683.28</v>
+        <v>263762.46000000002</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44231</v>
+        <v>44220</v>
       </c>
       <c r="B22" s="2">
-        <v>26376.25</v>
+        <v>-193326.38</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2">
-        <v>263762.46000000002</v>
+        <v>237386.21</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>44220</v>
-      </c>
-      <c r="B23" s="2">
-        <v>-193326.38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>237386.21</v>
-      </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>